<commit_message>
Add new maximum stock level column to stock offtake report
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/stockOfftakeReport.xlsx
+++ b/src/main/resources/excel/stockOfftakeReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>CODE</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>QUANTITY</t>
+  </si>
+  <si>
+    <t>NEW MAXIMUM STOCK LEVEL</t>
   </si>
 </sst>
 </file>
@@ -374,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -387,9 +390,10 @@
     <col min="3" max="3" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -403,6 +407,9 @@
         <v>3</v>
       </c>
       <c r="E1" s="2"/>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>